<commit_message>
User View -> Bulk User - users data array
</commit_message>
<xml_diff>
--- a/src/assets/xl/users(bulk).xlsx
+++ b/src/assets/xl/users(bulk).xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAMS\CAMS_NEW_GUI\src\assets\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C719426-2B63-48C3-AD31-429FE0E01FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A729B73-B5AE-44C5-B257-BA869A852863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1860" windowWidth="15180" windowHeight="9600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
     <sheet name="UserRoles" sheetId="2" r:id="rId2"/>
     <sheet name="Roles" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="roleCode">Roles!$A$2:$A$1048576</definedName>
+    <definedName name="users">UserInfo!$A$2:$A$1048576</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>First Name</t>
   </si>
@@ -50,20 +54,50 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Facility Manager (AES)</t>
-  </si>
-  <si>
-    <t>Facility Manager - TBS</t>
+    <t>AES - Admin AES</t>
+  </si>
+  <si>
+    <t>AES - Admin</t>
+  </si>
+  <si>
+    <t>TBS - Admin TBS</t>
+  </si>
+  <si>
+    <t>TBS - Tenant</t>
+  </si>
+  <si>
+    <t>C150</t>
+  </si>
+  <si>
+    <t>C151</t>
+  </si>
+  <si>
+    <t>C152</t>
+  </si>
+  <si>
+    <t>Role Code</t>
+  </si>
+  <si>
+    <t>Platform - Role</t>
+  </si>
+  <si>
+    <t>C153</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,7 +407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -405,6 +441,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -414,7 +451,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,33 +468,69 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{CB24B534-1172-447D-84A4-560207EB7E62}">
+      <formula1>users</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{E84DF5EE-392A-4E6B-96E3-48D370B6576D}">
+      <formula1>roleCode</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F41EF1-6519-490B-BF52-3A10C127FBEE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>150</v>
+      <c r="A1" t="s">
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>151</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Activity Logs -> Export
</commit_message>
<xml_diff>
--- a/src/assets/xl/users(bulk).xlsx
+++ b/src/assets/xl/users(bulk).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAMS\CAMS_NEW_GUI\src\assets\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A729B73-B5AE-44C5-B257-BA869A852863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429AD664-BA37-4960-B242-BCA52B78C79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5715" yWindow="2805" windowWidth="15180" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F41EF1-6519-490B-BF52-3A10C127FBEE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix bugs in upload user bulk
</commit_message>
<xml_diff>
--- a/src/assets/xl/users(bulk).xlsx
+++ b/src/assets/xl/users(bulk).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAMS\CAMS_NEW_GUI\src\assets\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kameera\Codes\frontend\CAMS_NEW_GUI\src\assets\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429AD664-BA37-4960-B242-BCA52B78C79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="2805" windowWidth="15180" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5715" yWindow="2805" windowWidth="15180" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
@@ -33,15 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -82,12 +72,21 @@
   </si>
   <si>
     <t>C153</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,11 +403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,22 +421,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE4C4C3-6AD5-4AD7-AF58-952D70CBF6F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -461,18 +460,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{CB24B534-1172-447D-84A4-560207EB7E62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>users</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{E84DF5EE-392A-4E6B-96E3-48D370B6576D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>roleCode</formula1>
     </dataValidation>
   </dataValidations>
@@ -481,7 +480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F41EF1-6519-490B-BF52-3A10C127FBEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -496,42 +495,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>